<commit_message>
DataPivot 과제 완료 0328
</commit_message>
<xml_diff>
--- a/07DataPivot/excel_data/가.xlsx
+++ b/07DataPivot/excel_data/가.xlsx
@@ -1,27 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ICT CoC\Documents\UiPath\RPA\07DataPivot\excel_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4sooh\Documents\UiPath\RPA수업\07DataPivot\excel_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F824E37E-F1B9-4CA6-BD66-3705634A38E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11295" yWindow="345" windowWidth="14955" windowHeight="15255" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11292" yWindow="348" windowWidth="14952" windowHeight="15252"/>
   </bookViews>
   <sheets>
-    <sheet name="가" sheetId="6" r:id="rId1"/>
-    <sheet name="가Summary" sheetId="5" r:id="rId2"/>
-    <sheet name="Summary" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
+    <sheet name="Summary" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="65" r:id="rId5"/>
-    <pivotCache cacheId="69" r:id="rId6"/>
+    <pivotCache cacheId="237" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="27">
   <si>
     <t>번호</t>
   </si>
@@ -113,9 +109,6 @@
   </si>
   <si>
     <t>행 레이블</t>
-  </si>
-  <si>
-    <t>(비어 있음)</t>
   </si>
   <si>
     <t>총합계</t>
@@ -127,7 +120,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="&quot;₩&quot;#,##0_);[Red]\(&quot;₩&quot;#,##0\)"/>
   </numFmts>
@@ -212,80 +205,35 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="ICT CoC" refreshedDate="45378.620481597223" createdVersion="1" refreshedVersion="6" recordCount="31" xr:uid="{1F590BED-1294-4343-A565-F0C5F20E62FA}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="4sooha@naver.com" refreshedDate="45379.949076620367" createdVersion="1" refreshedVersion="5" recordCount="30">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:G1048576" sheet="Sheet1"/>
+    <worksheetSource ref="A1:G31" sheet="Sheet1"/>
   </cacheSource>
   <cacheFields count="7">
     <cacheField name="번호" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="30"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="30"/>
     </cacheField>
     <cacheField name="품명" numFmtId="0">
-      <sharedItems containsBlank="1" count="7">
+      <sharedItems count="6">
         <s v="라이언"/>
         <s v="프로도"/>
         <s v="네오"/>
         <s v="콘"/>
         <s v="무지"/>
         <s v="튜브"/>
-        <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="본부" numFmtId="0">
-      <sharedItems containsBlank="1"/>
+      <sharedItems/>
     </cacheField>
-    <cacheField name="WBS번호" numFmtId="0">
-      <sharedItems containsBlank="1"/>
+    <cacheField name="WBS번호" numFmtId="49">
+      <sharedItems/>
     </cacheField>
-    <cacheField name="만기일" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-08-31T00:00:00" maxDate="2019-09-01T00:00:00"/>
+    <cacheField name="만기일" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2019-08-31T00:00:00" maxDate="2019-09-01T00:00:00"/>
     </cacheField>
-    <cacheField name="금액" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="15060" maxValue="994284"/>
-    </cacheField>
-    <cacheField name="비고" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="ICT CoC" refreshedDate="45378.653109722225" createdVersion="1" refreshedVersion="6" recordCount="31" xr:uid="{DCCDA7D5-3A0D-42D0-93D9-0B8D13AC91C1}">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A1:G1048576" sheet="Sheet1"/>
-  </cacheSource>
-  <cacheFields count="7">
-    <cacheField name="번호" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="30"/>
-    </cacheField>
-    <cacheField name="품명" numFmtId="0">
-      <sharedItems containsBlank="1" count="7">
-        <s v="라이언"/>
-        <s v="프로도"/>
-        <s v="네오"/>
-        <s v="콘"/>
-        <s v="무지"/>
-        <s v="튜브"/>
-        <m/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="본부" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="WBS번호" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="만기일" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-08-31T00:00:00" maxDate="2019-09-01T00:00:00"/>
-    </cacheField>
-    <cacheField name="금액" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="15060" maxValue="994284"/>
+    <cacheField name="금액" numFmtId="176">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="15060" maxValue="994284"/>
     </cacheField>
     <cacheField name="비고" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
@@ -300,7 +248,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="31">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="30">
   <r>
     <n v="1"/>
     <x v="0"/>
@@ -571,305 +519,12 @@
     <n v="708593"/>
     <m/>
   </r>
-  <r>
-    <m/>
-    <x v="6"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="31">
-  <r>
-    <n v="1"/>
-    <x v="0"/>
-    <s v="본사"/>
-    <s v="L10N-3215"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="49926"/>
-    <m/>
-  </r>
-  <r>
-    <n v="2"/>
-    <x v="1"/>
-    <s v="인천"/>
-    <s v="FR0DO-715"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="408731"/>
-    <m/>
-  </r>
-  <r>
-    <n v="3"/>
-    <x v="2"/>
-    <s v="부산"/>
-    <s v="NE0-6154"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="245111"/>
-    <m/>
-  </r>
-  <r>
-    <n v="4"/>
-    <x v="3"/>
-    <s v="대전"/>
-    <s v="C0N-319"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="603915"/>
-    <m/>
-  </r>
-  <r>
-    <n v="5"/>
-    <x v="1"/>
-    <s v="인천"/>
-    <s v="FR0DO-715"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="440295"/>
-    <m/>
-  </r>
-  <r>
-    <n v="6"/>
-    <x v="4"/>
-    <s v="대전"/>
-    <s v="MUZ1-877"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="799100"/>
-    <m/>
-  </r>
-  <r>
-    <n v="7"/>
-    <x v="0"/>
-    <s v="본사"/>
-    <s v="L10N-3215"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="157906"/>
-    <m/>
-  </r>
-  <r>
-    <n v="8"/>
-    <x v="5"/>
-    <s v="대구"/>
-    <s v="Y0U-TUBE"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="994284"/>
-    <m/>
-  </r>
-  <r>
-    <n v="9"/>
-    <x v="1"/>
-    <s v="부산"/>
-    <s v="FR0DO-715"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="353090"/>
-    <m/>
-  </r>
-  <r>
-    <n v="10"/>
-    <x v="4"/>
-    <s v="대전"/>
-    <s v="MUZ1-877"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="711895"/>
-    <m/>
-  </r>
-  <r>
-    <n v="11"/>
-    <x v="3"/>
-    <s v="인천"/>
-    <s v="C0N-319"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="548275"/>
-    <m/>
-  </r>
-  <r>
-    <n v="12"/>
-    <x v="5"/>
-    <s v="대구"/>
-    <s v="Y0U-TUBE"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="907079"/>
-    <m/>
-  </r>
-  <r>
-    <n v="13"/>
-    <x v="4"/>
-    <s v="대전"/>
-    <s v="MUZ1-877"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="743459"/>
-    <m/>
-  </r>
-  <r>
-    <n v="14"/>
-    <x v="4"/>
-    <s v="본사"/>
-    <s v="MUZ1-877"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="102265"/>
-    <m/>
-  </r>
-  <r>
-    <n v="15"/>
-    <x v="1"/>
-    <s v="인천"/>
-    <s v="FR0DO-715"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="461070"/>
-    <m/>
-  </r>
-  <r>
-    <n v="16"/>
-    <x v="2"/>
-    <s v="부산"/>
-    <s v="NE0-6154"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="297449"/>
-    <m/>
-  </r>
-  <r>
-    <n v="17"/>
-    <x v="3"/>
-    <s v="대전"/>
-    <s v="C0N-319"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="656254"/>
-    <m/>
-  </r>
-  <r>
-    <n v="18"/>
-    <x v="0"/>
-    <s v="본사"/>
-    <s v="L10N-3215"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="15060"/>
-    <m/>
-  </r>
-  <r>
-    <n v="19"/>
-    <x v="5"/>
-    <s v="대구"/>
-    <s v="Y0U-TUBE"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="851439"/>
-    <m/>
-  </r>
-  <r>
-    <n v="20"/>
-    <x v="2"/>
-    <s v="부산"/>
-    <s v="NE0-6154"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="210244"/>
-    <m/>
-  </r>
-  <r>
-    <n v="21"/>
-    <x v="0"/>
-    <s v="본사"/>
-    <s v="L10N-3215"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="46624"/>
-    <m/>
-  </r>
-  <r>
-    <n v="22"/>
-    <x v="1"/>
-    <s v="인천"/>
-    <s v="FR0DO-715"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="405429"/>
-    <m/>
-  </r>
-  <r>
-    <n v="23"/>
-    <x v="4"/>
-    <s v="대전"/>
-    <s v="MUZ1-877"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="764234"/>
-    <m/>
-  </r>
-  <r>
-    <n v="24"/>
-    <x v="3"/>
-    <s v="대전"/>
-    <s v="C0N-319"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="600613"/>
-    <m/>
-  </r>
-  <r>
-    <n v="25"/>
-    <x v="5"/>
-    <s v="대구"/>
-    <s v="Y0U-TUBE"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="959418"/>
-    <m/>
-  </r>
-  <r>
-    <n v="26"/>
-    <x v="2"/>
-    <s v="부산"/>
-    <s v="NE0-6154"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="318224"/>
-    <m/>
-  </r>
-  <r>
-    <n v="27"/>
-    <x v="0"/>
-    <s v="본사"/>
-    <s v="L10N-3215"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="154604"/>
-    <m/>
-  </r>
-  <r>
-    <n v="28"/>
-    <x v="3"/>
-    <s v="인천"/>
-    <s v="C0N-319"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="513408"/>
-    <m/>
-  </r>
-  <r>
-    <n v="29"/>
-    <x v="1"/>
-    <s v="부산"/>
-    <s v="FR0DO-715"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="349788"/>
-    <m/>
-  </r>
-  <r>
-    <n v="30"/>
-    <x v="4"/>
-    <s v="대전"/>
-    <s v="MUZ1-877"/>
-    <d v="2019-08-31T00:00:00"/>
-    <n v="708593"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <x v="6"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2C60B9EC-AB31-4EAD-8C25-B310CF640F82}" name="가Summary" cacheId="65" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="데이터" updatedVersion="6" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1">
-  <location ref="A1:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Summary" cacheId="237" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="데이터" updatedVersion="5" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1">
+  <location ref="A1:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0" includeNewItemsInFilter="1">
       <extLst>
@@ -879,14 +534,13 @@
       </extLst>
     </pivotField>
     <pivotField axis="axisRow" showAll="0" includeNewItemsInFilter="1">
-      <items count="8">
+      <items count="7">
         <item x="2"/>
         <item x="0"/>
         <item x="4"/>
         <item x="3"/>
         <item x="5"/>
         <item x="1"/>
-        <item x="6"/>
         <item t="default"/>
       </items>
       <extLst>
@@ -909,14 +563,14 @@
         </ext>
       </extLst>
     </pivotField>
-    <pivotField showAll="0" includeNewItemsInFilter="1">
+    <pivotField numFmtId="14" showAll="0" includeNewItemsInFilter="1">
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
           <x14:pivotField fillDownLabels="1"/>
         </ext>
       </extLst>
     </pivotField>
-    <pivotField dataField="1" showAll="0" includeNewItemsInFilter="1">
+    <pivotField dataField="1" numFmtId="176" showAll="0" includeNewItemsInFilter="1">
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
           <x14:pivotField fillDownLabels="1"/>
@@ -934,7 +588,7 @@
   <rowFields count="1">
     <field x="1"/>
   </rowFields>
-  <rowItems count="8">
+  <rowItems count="7">
     <i>
       <x/>
     </i>
@@ -953,9 +607,6 @@
     <i>
       <x v="5"/>
     </i>
-    <i>
-      <x v="6"/>
-    </i>
     <i t="grand">
       <x/>
     </i>
@@ -970,120 +621,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6FCC79F8-20D5-47F9-B056-3DB14843DE31}" name="Summary" cacheId="69" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="데이터" updatedVersion="6" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1">
-  <location ref="A1:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0" includeNewItemsInFilter="1">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" includeNewItemsInFilter="1">
-      <items count="8">
-        <item x="2"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField showAll="0" includeNewItemsInFilter="1">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField showAll="0" includeNewItemsInFilter="1">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField showAll="0" includeNewItemsInFilter="1">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField dataField="1" showAll="0" includeNewItemsInFilter="1">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField showAll="0" includeNewItemsInFilter="1">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="8">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="합계 : 금액" fld="5" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
     </ext>
   </extLst>
 </pivotTableDefinition>
@@ -1351,309 +888,109 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC45F80-47F1-490B-B836-A32D7BB0C3D5}">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1">
+      <c r="B2" s="1">
         <v>1071028</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B2">
+      <c r="B3" s="1">
         <v>424120</v>
       </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3">
+      <c r="B4" s="1">
         <v>3829546</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B5" s="1">
         <v>2922465</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
+      <c r="B6" s="1">
         <v>3712220</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6">
+      <c r="B7" s="1">
         <v>2418403</v>
       </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>14377782</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C28FD1-C0CE-4858-9F87-2BF702AEF538}">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1071028</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="1">
-        <v>424120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3829546</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2922465</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1">
-        <v>3712220</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2418403</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="1">
-        <v>14377782</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1071028</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="1">
-        <v>424120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3829546</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2922465</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1">
-        <v>3712220</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2418403</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="1">
-        <v>14377782</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="4" max="4" width="10.625" customWidth="1"/>
-    <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.59765625" customWidth="1"/>
+    <col min="5" max="5" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.69921875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="11.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1676,7 +1013,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1702,7 +1039,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1728,7 +1065,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1754,7 +1091,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1780,7 +1117,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1806,7 +1143,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -1832,7 +1169,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -1858,7 +1195,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -1884,7 +1221,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -1910,7 +1247,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -1936,7 +1273,7 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -1962,7 +1299,7 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -1988,7 +1325,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -2014,7 +1351,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -2040,7 +1377,7 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -2066,7 +1403,7 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -2092,7 +1429,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -2118,7 +1455,7 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -2144,7 +1481,7 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -2170,7 +1507,7 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -2196,7 +1533,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -2222,7 +1559,7 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -2248,7 +1585,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -2274,7 +1611,7 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -2300,7 +1637,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -2326,7 +1663,7 @@
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -2347,7 +1684,7 @@
       </c>
       <c r="G27" s="10"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -2368,7 +1705,7 @@
       </c>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -2389,7 +1726,7 @@
       </c>
       <c r="G29" s="10"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -2410,7 +1747,7 @@
       </c>
       <c r="G30" s="10"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" s="6">
         <v>30</v>
       </c>

</xml_diff>